<commit_message>
changed to correct new diagrams in handin and fixed integration plan
</commit_message>
<xml_diff>
--- a/Integrationsplan.xlsx
+++ b/Integrationsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anders Fibiger\Documents\4_semester\AirTrafficMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FF2D62-7145-41BB-872C-A41C01C65E1A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47481F-9652-49CA-9FBF-D4238D542955}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{88F05436-07DD-411A-A269-36F08A646B80}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>Step</t>
   </si>
@@ -118,8 +118,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14E2A777-AE40-4F26-94A8-191BF2B6FB28}" name="Tabel3" displayName="Tabel3" ref="A1:H8" totalsRowShown="0">
-  <autoFilter ref="A1:H8" xr:uid="{61418946-0A12-4BA8-84CB-D029348563E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14E2A777-AE40-4F26-94A8-191BF2B6FB28}" name="Tabel3" displayName="Tabel3" ref="A1:H7" totalsRowShown="0">
+  <autoFilter ref="A1:H7" xr:uid="{61418946-0A12-4BA8-84CB-D029348563E7}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E34659B4-F642-4A92-A977-A1FE056A0004}" name="Step"/>
     <tableColumn id="2" xr3:uid="{A9E1C44D-8449-4D65-B563-ADE02A95942B}" name="TransponderReceiver"/>
@@ -431,21 +431,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9487531C-C25E-4AEF-BFB7-FB3F7A9B32B7}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -479,10 +479,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -490,10 +499,19 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
+      <c r="H3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -501,10 +519,19 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -512,10 +539,19 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -523,10 +559,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -546,10 +582,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -564,32 +600,6 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed integration plan according to bottom up using dependency tree
</commit_message>
<xml_diff>
--- a/Integrationsplan.xlsx
+++ b/Integrationsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anders Fibiger\Documents\4_semester\AirTrafficMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47481F-9652-49CA-9FBF-D4238D542955}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15AF83-1B6B-4223-9C44-4F6FAB04604D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{88F05436-07DD-411A-A269-36F08A646B80}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="4452" xr2:uid="{88F05436-07DD-411A-A269-36F08A646B80}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Step</t>
   </si>
@@ -118,8 +118,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14E2A777-AE40-4F26-94A8-191BF2B6FB28}" name="Tabel3" displayName="Tabel3" ref="A1:H7" totalsRowShown="0">
-  <autoFilter ref="A1:H7" xr:uid="{61418946-0A12-4BA8-84CB-D029348563E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14E2A777-AE40-4F26-94A8-191BF2B6FB28}" name="Tabel3" displayName="Tabel3" ref="A1:H4" totalsRowShown="0">
+  <autoFilter ref="A1:H4" xr:uid="{61418946-0A12-4BA8-84CB-D029348563E7}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E34659B4-F642-4A92-A977-A1FE056A0004}" name="Step"/>
     <tableColumn id="2" xr3:uid="{A9E1C44D-8449-4D65-B563-ADE02A95942B}" name="TransponderReceiver"/>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9487531C-C25E-4AEF-BFB7-FB3F7A9B32B7}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,6 +478,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
@@ -485,21 +488,24 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -508,18 +514,24 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -531,75 +543,6 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final changes to handin
</commit_message>
<xml_diff>
--- a/Integrationsplan.xlsx
+++ b/Integrationsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anders Fibiger\Documents\4_semester\AirTrafficMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15AF83-1B6B-4223-9C44-4F6FAB04604D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFB5197-0F6A-46AE-BA4B-1F4D41C3328E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="4452" xr2:uid="{88F05436-07DD-411A-A269-36F08A646B80}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t>Step</t>
   </si>
@@ -434,7 +434,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,6 +501,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>

</xml_diff>